<commit_message>
Final update from me
</commit_message>
<xml_diff>
--- a/fst-ueb4.xlsx
+++ b/fst-ueb4.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
   <si>
     <r>
       <t xml:space="preserve">Allg Datenstruktur für </t>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>addToTail(int value)</t>
-  </si>
-  <si>
-    <t>fertig</t>
   </si>
   <si>
     <t>length()</t>
@@ -471,8 +468,8 @@
   </sheetPr>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -649,16 +646,14 @@
         <v>22</v>
       </c>
       <c r="E22" s="8"/>
-      <c r="F22" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>21</v>
@@ -667,16 +662,14 @@
         <v>22</v>
       </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>25</v>
@@ -690,13 +683,13 @@
         <v>7</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,7 +697,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>21</v>
@@ -713,7 +706,7 @@
         <v>26</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -721,16 +714,16 @@
         <v>9</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>25</v>
@@ -747,16 +740,14 @@
         <v>22</v>
       </c>
       <c r="E28" s="8"/>
-      <c r="F28" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>25</v>
@@ -770,16 +761,16 @@
         <v>12</v>
       </c>
       <c r="B30" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,10 +778,10 @@
         <v>13</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>26</v>
@@ -801,16 +792,16 @@
         <v>14</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F32" s="4"/>
     </row>
@@ -819,18 +810,19 @@
         <v>15</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,7 +830,7 @@
         <v>15</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,12 +846,12 @@
         <v>2</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,17 +859,17 @@
         <v>3</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,17 +877,17 @@
         <v>4</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,12 +895,12 @@
         <v>5</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,22 +908,22 @@
         <v>6</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>